<commit_message>
Se agregan los campos de validadcion : Comprobante, fecha vencimiento y codigo cvc a la question SolicitudEprepago, se refactoriza el feature descargartarjetavirtualeprepago
</commit_message>
<xml_diff>
--- a/APP_PERSONAS/src/test/resources/datadriven/e-prepago/descargar_tarjeta_virtual_eprepago.xlsx
+++ b/APP_PERSONAS/src/test/resources/datadriven/e-prepago/descargar_tarjeta_virtual_eprepago.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\appOPS\bancolombia-app-personas-osp-tests-bdd-screen-play\APP_PERSONAS\src\test\resources\datadriven\e-prepago\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\appOSP\bancolombia-app-personas-osp-tests-bdd-screen-play\APP_PERSONAS\src\test\resources\datadriven\e-prepago\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B93CB4EF-B5A5-47EE-AF56-672FC83C17B0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F4DB2EF-4BBE-4BE0-9B66-1D34285E0B60}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>ID</t>
   </si>
@@ -73,15 +73,6 @@
   </si>
   <si>
     <t>ACTIVO</t>
-  </si>
-  <si>
-    <t>valorDescarga</t>
-  </si>
-  <si>
-    <t>opcionSubmenu</t>
-  </si>
-  <si>
-    <t>Descargar</t>
   </si>
   <si>
     <t>pruebasregistro49</t>
@@ -422,7 +413,7 @@
   <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="M1" sqref="M1:N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -467,12 +458,8 @@
       <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>17</v>
-      </c>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
       <c r="O1" s="2"/>
     </row>
     <row r="2" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
@@ -486,7 +473,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E2" s="1">
         <v>1234</v>
@@ -512,12 +499,8 @@
       <c r="L2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="M2" s="1">
-        <v>10000</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>18</v>
-      </c>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Se refactoriza el feature descargar_tarjeta_virtual_e_prepago, se refactoriza el nombre de la tarea DescargarSaldo
</commit_message>
<xml_diff>
--- a/APP_PERSONAS/src/test/resources/datadriven/e-prepago/descargar_tarjeta_virtual_eprepago.xlsx
+++ b/APP_PERSONAS/src/test/resources/datadriven/e-prepago/descargar_tarjeta_virtual_eprepago.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\appOSP\bancolombia-app-personas-osp-tests-bdd-screen-play\APP_PERSONAS\src\test\resources\datadriven\e-prepago\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F4DB2EF-4BBE-4BE0-9B66-1D34285E0B60}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A129ABC3-96C7-4D71-A6ED-BBF67073C1DD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Datos" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="27">
   <si>
     <t>ID</t>
   </si>
@@ -75,14 +75,44 @@
     <t>ACTIVO</t>
   </si>
   <si>
-    <t>pruebasregistro49</t>
+    <t>valorRecarga</t>
+  </si>
+  <si>
+    <t>tipoCuenta</t>
+  </si>
+  <si>
+    <t>numeroCuenta</t>
+  </si>
+  <si>
+    <t>autotest32</t>
+  </si>
+  <si>
+    <t>000</t>
+  </si>
+  <si>
+    <t>0369</t>
+  </si>
+  <si>
+    <t>10.000</t>
+  </si>
+  <si>
+    <t>Ahorros</t>
+  </si>
+  <si>
+    <t>406-733040-20</t>
+  </si>
+  <si>
+    <t>autotest25</t>
+  </si>
+  <si>
+    <t>406-739740-05</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -100,24 +130,61 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <color indexed="8"/>
+      <name val="Mic Shell Dlg"/>
+      <charset val="134"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -126,10 +193,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -410,19 +485,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O2"/>
+  <dimension ref="A1:O3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1:N2"/>
+      <selection activeCell="O1" sqref="O1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
   <cols>
     <col min="2" max="2" width="18.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:15" ht="15">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -440,16 +515,16 @@
       <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
       <c r="K1" s="2" t="s">
@@ -458,49 +533,109 @@
       <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
+      <c r="M1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="2" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="1">
+    <row r="2" spans="1:15" ht="15.5">
+      <c r="A2" s="4">
         <v>1</v>
       </c>
-      <c r="B2" s="1">
-        <v>93221451</v>
-      </c>
-      <c r="C2" s="1">
+      <c r="B2" s="4">
+        <v>333333304</v>
+      </c>
+      <c r="C2" s="4">
         <v>1</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" s="1">
+      <c r="D2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" s="4">
         <v>1234</v>
       </c>
-      <c r="F2" s="1">
+      <c r="F2" s="4">
         <v>4321</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="H2" s="1">
-        <v>0</v>
-      </c>
-      <c r="I2" s="1">
-        <v>369</v>
-      </c>
-      <c r="J2" s="1" t="s">
+      <c r="H2" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="J2" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="K2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="L2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="M2" s="1"/>
-      <c r="N2" s="1"/>
+      <c r="M2" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" ht="15.5">
+      <c r="A3" s="4">
+        <v>1</v>
+      </c>
+      <c r="B3" s="4">
+        <v>93221450</v>
+      </c>
+      <c r="C3" s="4">
+        <v>1</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" s="4">
+        <v>1234</v>
+      </c>
+      <c r="F3" s="4">
+        <v>4321</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="M3" s="6">
+        <v>3000000</v>
+      </c>
+      <c r="N3" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="O3" s="4" t="s">
+        <v>26</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Se crea la clase Question DescargaTarjetaVirtuaEprepago para validar la descarga de la tarjeta virtual ePrepago
</commit_message>
<xml_diff>
--- a/APP_PERSONAS/src/test/resources/datadriven/e-prepago/descargar_tarjeta_virtual_eprepago.xlsx
+++ b/APP_PERSONAS/src/test/resources/datadriven/e-prepago/descargar_tarjeta_virtual_eprepago.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\appOSP\bancolombia-app-personas-osp-tests-bdd-screen-play\APP_PERSONAS\src\test\resources\datadriven\e-prepago\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A129ABC3-96C7-4D71-A6ED-BBF67073C1DD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DAF4881-2770-4802-9266-D3F252F94D0E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -75,9 +75,6 @@
     <t>ACTIVO</t>
   </si>
   <si>
-    <t>valorRecarga</t>
-  </si>
-  <si>
     <t>tipoCuenta</t>
   </si>
   <si>
@@ -106,6 +103,9 @@
   </si>
   <si>
     <t>406-739740-05</t>
+  </si>
+  <si>
+    <t>valorDescarga</t>
   </si>
 </sst>
 </file>
@@ -488,7 +488,7 @@
   <dimension ref="A1:O3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O1" sqref="O1"/>
+      <selection activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
@@ -534,13 +534,13 @@
         <v>11</v>
       </c>
       <c r="M1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="N1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>17</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="15.5">
@@ -554,7 +554,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E2" s="4">
         <v>1234</v>
@@ -566,10 +566,10 @@
         <v>12</v>
       </c>
       <c r="H2" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="I2" s="5" t="s">
         <v>20</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>21</v>
       </c>
       <c r="J2" s="4" t="s">
         <v>13</v>
@@ -581,13 +581,13 @@
         <v>15</v>
       </c>
       <c r="M2" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="N2" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="N2" s="4" t="s">
+      <c r="O2" s="4" t="s">
         <v>23</v>
-      </c>
-      <c r="O2" s="4" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="15.5">
@@ -601,7 +601,7 @@
         <v>1</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E3" s="4">
         <v>1234</v>
@@ -613,10 +613,10 @@
         <v>12</v>
       </c>
       <c r="H3" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="I3" s="5" t="s">
         <v>20</v>
-      </c>
-      <c r="I3" s="5" t="s">
-        <v>21</v>
       </c>
       <c r="J3" s="4" t="s">
         <v>13</v>
@@ -631,10 +631,10 @@
         <v>3000000</v>
       </c>
       <c r="N3" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="O3" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Refactorización clase question DescargaTarjetaVirtuaEprepago
</commit_message>
<xml_diff>
--- a/APP_PERSONAS/src/test/resources/datadriven/e-prepago/descargar_tarjeta_virtual_eprepago.xlsx
+++ b/APP_PERSONAS/src/test/resources/datadriven/e-prepago/descargar_tarjeta_virtual_eprepago.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\appOSP\bancolombia-app-personas-osp-tests-bdd-screen-play\APP_PERSONAS\src\test\resources\datadriven\e-prepago\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31F1C13D-5A3C-4C60-A3B6-1F592F1F0310}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34CED967-0290-4A8D-A731-EC75A507FD78}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -99,13 +99,13 @@
     <t>valorDescarga</t>
   </si>
   <si>
-    <t>5000</t>
-  </si>
-  <si>
     <t>autotest32</t>
   </si>
   <si>
     <t>406-733040-20</t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
 </sst>
 </file>
@@ -488,7 +488,7 @@
   <dimension ref="A1:O3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
@@ -554,7 +554,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E2" s="4">
         <v>1234</v>
@@ -581,13 +581,13 @@
         <v>15</v>
       </c>
       <c r="M2" s="6" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="N2" s="4" t="s">
         <v>20</v>
       </c>
       <c r="O2" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="15.5">

</xml_diff>